<commit_message>
update trad and label database (encore)
</commit_message>
<xml_diff>
--- a/tests/label.xlsx
+++ b/tests/label.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\141187\Documents\GitHub\ermeeth\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3362ADE4-6AAD-4EDA-92B5-104431946BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C8EE0-8101-485A-A0A6-E8F7BFC16CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -82,45 +82,24 @@
     <t>I_SNF</t>
   </si>
   <si>
-    <t>Investissement des SNF et EI</t>
-  </si>
-  <si>
     <t>PYM</t>
   </si>
   <si>
-    <t>Prix de production marchande</t>
-  </si>
-  <si>
     <t>PCI</t>
   </si>
   <si>
-    <t>Prix de CI</t>
-  </si>
-  <si>
     <t>C_L</t>
   </si>
   <si>
-    <t>Coût réel du travail</t>
-  </si>
-  <si>
     <t>F_L_Q</t>
   </si>
   <si>
-    <t>Emploi qualifié (en milliers)</t>
-  </si>
-  <si>
     <t>F_L_NQ</t>
   </si>
   <si>
-    <t>Emploi non qualifié (en milliers)</t>
-  </si>
-  <si>
     <t>VA_SM</t>
   </si>
   <si>
-    <t>VA du secteur marchand</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -196,10 +175,31 @@
     <t>F_L_SM</t>
   </si>
   <si>
-    <t>Employment (commercial sector)</t>
-  </si>
-  <si>
     <t>RBAL_TRADE_VAL</t>
+  </si>
+  <si>
+    <t>Employment in thousands (commercial sector)</t>
+  </si>
+  <si>
+    <t>Non-qualified employment (in thousands)</t>
+  </si>
+  <si>
+    <t>Qualified employment (in thousands)</t>
+  </si>
+  <si>
+    <t>VA (commercial sector)</t>
+  </si>
+  <si>
+    <t>Production price (commercial sector)</t>
+  </si>
+  <si>
+    <t>Investment (SNF + EI)</t>
+  </si>
+  <si>
+    <t>Cost of labor</t>
+  </si>
+  <si>
+    <t>Intermediate consumption price</t>
   </si>
 </sst>
 </file>
@@ -535,17 +535,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,23 +553,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -577,7 +577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -585,7 +585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -593,55 +593,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -649,15 +649,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -665,23 +665,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -689,7 +689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -697,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -705,84 +705,84 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
       <c r="B26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update trad and label
</commit_message>
<xml_diff>
--- a/tests/label.xlsx
+++ b/tests/label.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\141187\Documents\GitHub\ermeeth\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193C8EE0-8101-485A-A0A6-E8F7BFC16CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262A25EC-682D-412C-9BB1-128B93E19B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>DISPINC_AT</t>
   </si>
   <si>
-    <t>Household disposable income</t>
-  </si>
-  <si>
     <t>I_SNF</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Intermediate consumption price</t>
+  </si>
+  <si>
+    <t>Household real disposable income</t>
   </si>
 </sst>
 </file>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,18 +555,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,50 +595,50 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,10 +651,10 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,18 +667,18 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
         <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -707,82 +707,82 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
         <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" t="s">
         <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
         <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
         <v>27</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>